<commit_message>
Evaluation of conditional formatting if cell is empty - Added test of CF based on numeric formula in a empty cell (#32)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -471,7 +471,125 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -777,7 +895,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -864,13 +982,33 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="9" priority="5">
       <formula>($A$1=A2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="7" priority="3">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" dxfId="5" priority="1">
+      <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,6 +1042,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -20061,35 +20208,26 @@
 </easyPacket>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Rebase with 1.3 and Added a test for cell borders (#39)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="195" yWindow="90" windowWidth="18390" windowHeight="7545" activeTab="1"/>
+    <workbookView xWindow="195" yWindow="90" windowWidth="18390" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -155,7 +155,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +192,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -315,6 +321,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -413,7 +471,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -422,6 +480,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="%0." xfId="4"/>
@@ -471,7 +534,45 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -483,6 +584,21 @@
       <font>
         <color theme="0"/>
       </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -761,13 +877,30 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1"/>
+  <dimension ref="C7:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="8">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C7:D7">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -776,8 +909,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" showZeros="0" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -828,12 +961,23 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="6">
+        <v>22</v>
+      </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
@@ -864,13 +1008,38 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="1" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>($A$1=A2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A10">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B10">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D10">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -904,6 +1073,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -20061,35 +20239,26 @@
 </easyPacket>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added test for conditional formatting about cell borders (#39)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -42,12 +42,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00,"/>
-    <numFmt numFmtId="166" formatCode="#,##0,"/>
-    <numFmt numFmtId="167" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0_-;\-&quot;€&quot;\ * #,##0_-;_-&quot;€&quot;\ * &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00,"/>
+    <numFmt numFmtId="168" formatCode="#,##0,"/>
+    <numFmt numFmtId="169" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="15" x14ac:knownFonts="1">
     <font>
@@ -155,7 +155,7 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -192,8 +192,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -315,16 +321,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="167" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -343,20 +364,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
+    <xf numFmtId="168" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyFill="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="9" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0">
@@ -376,7 +397,7 @@
     <xf numFmtId="37" fontId="9" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
+    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
@@ -389,7 +410,7 @@
     <xf numFmtId="9" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="6" borderId="8" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
+    <xf numFmtId="167" fontId="6" fillId="6" borderId="8" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment horizontal="right"/>
     </xf>
@@ -413,7 +434,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -422,6 +443,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="%0." xfId="4"/>
@@ -471,39 +494,42 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="15">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -546,6 +572,14 @@
       </font>
     </dxf>
     <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
@@ -562,14 +596,9 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -577,18 +606,6 @@
           <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <fill>
@@ -895,7 +912,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -952,12 +969,25 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5">
+        <v>12</v>
+      </c>
+      <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4">
+        <v>10</v>
+      </c>
+      <c r="E16" s="4"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -982,33 +1012,43 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="10" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="9" priority="5">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>($A$1=A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="7" priority="3">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>-1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D15">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>12</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1042,15 +1082,6 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<easyPacket version="1.0">
-  <header version="5.2.3.0-SNAPSHOT"/>
-  <data>
-    <l refId="0" ln="0" eid="XLHiddenElement"/>
-  </data>
-</easyPacket>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <easyPacket version="1.0">
   <header version="5.2.3.0-SNAPSHOT"/>
   <data>
@@ -20208,26 +20239,35 @@
 </easyPacket>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<easyPacket version="1.0">
+  <header version="5.2.3.0-SNAPSHOT"/>
+  <data>
+    <l refId="0" ln="0" eid="XLHiddenElement"/>
+  </data>
+</easyPacket>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
+  <ds:schemaRefs/>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BACAB1D-108B-42D8-A647-601FA3A7ECC4}">
-  <ds:schemaRefs/>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20A5F204-C67D-477C-B772-C48FB5F2D05E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added conditional formatting tests with rules about the border style of cells (#39)
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -29,12 +29,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Foooooooooooo</t>
   </si>
   <si>
     <t>NotFoo</t>
+  </si>
+  <si>
+    <t>border</t>
+  </si>
+  <si>
+    <t>borderless</t>
+  </si>
+  <si>
+    <t>Step 2: Verify -&gt; D15 must not have borders</t>
+  </si>
+  <si>
+    <t>Step 3: Verify -&gt; D16 must have borders</t>
+  </si>
+  <si>
+    <t>Step 1: Verify -&gt; D14 must not have borders</t>
+  </si>
+  <si>
+    <t>Step 4: Verify -&gt; D16 must have borders</t>
+  </si>
+  <si>
+    <t>Step 5: Insert "borderless" in D16 -&gt; Borders disappear (only D16)</t>
+  </si>
+  <si>
+    <t>Step 6: Insert "borderless" in D14 -&gt; Only left border of D14 disappear</t>
   </si>
 </sst>
 </file>
@@ -440,11 +464,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="46">
     <cellStyle name="%0." xfId="4"/>
@@ -494,7 +518,7 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="15">
+  <dxfs count="7">
     <dxf>
       <border>
         <left style="thin">
@@ -512,64 +536,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
     <dxf>
       <border>
@@ -613,11 +579,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -911,28 +872,31 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -969,86 +933,99 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
       <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5">
-        <v>12</v>
+      <c r="B15" t="s">
+        <v>4</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="3"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
-        <v>10</v>
+      <c r="B16" t="s">
+        <v>5</v>
       </c>
-      <c r="E16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="13" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>($A$1=A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="12" priority="6">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="11" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="10" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="9" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
-      <formula>12</formula>
+  <conditionalFormatting sqref="D15 D14">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"borderless"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
-      <formula>10</formula>
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"border"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#39 Whitespace and typoes fixes
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\GIT\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="195" yWindow="90" windowWidth="18390" windowHeight="7545" activeTab="1"/>
+    <workbookView xWindow="12660" yWindow="660" windowWidth="26400" windowHeight="15740" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -19,9 +19,12 @@
     <definedName name="DOMESTIC">#REF!</definedName>
     <definedName name="INTL">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Foooooooooooo</t>
   </si>
@@ -43,22 +46,25 @@
     <t>borderless</t>
   </si>
   <si>
-    <t>Step 2: Verify -&gt; D15 must not have borders</t>
+    <t>Setup &amp; check:</t>
   </si>
   <si>
-    <t>Step 3: Verify -&gt; D16 must have borders</t>
+    <t>1) All cells in the red area have conditional formatting: on value "border" they have borders and on value "borderless" no border.</t>
   </si>
   <si>
-    <t>Step 1: Verify -&gt; D14 must not have borders</t>
+    <t>2) C14 and D15 have borders set as normal formatting</t>
   </si>
   <si>
-    <t>Step 4: Verify -&gt; D16 must have borders</t>
+    <t>3) "borderless" value in D15 makes the border to be hidden</t>
   </si>
   <si>
-    <t>Step 5: Insert "borderless" in D16 -&gt; Borders disappear (only D16)</t>
+    <t>5) Test by changing values, e.g. put "borderless" into D14 and check that left border disappears</t>
   </si>
   <si>
-    <t>Step 6: Insert "borderless" in D14 -&gt; Only left border of D14 disappear</t>
+    <t>6) In Excel the behavior is that conditional formatting takes precedence over normal formatting, and if both borderless and border are applied to adjacent cells, the common edge has a border.</t>
+  </si>
+  <si>
+    <t>4) "border" value in D16 makes a border appear.</t>
   </si>
 </sst>
 </file>
@@ -458,7 +464,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -468,6 +474,12 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="13" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="46">
@@ -488,8 +500,6 @@
     <cellStyle name="Bold+Italic" xfId="18"/>
     <cellStyle name="C_Amount_ACT" xfId="19"/>
     <cellStyle name="C_Head" xfId="20"/>
-    <cellStyle name="Currency" xfId="1" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Currency [0]" xfId="2" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Date" xfId="21"/>
     <cellStyle name="Fill light blue" xfId="22"/>
     <cellStyle name="Formula" xfId="23"/>
@@ -497,7 +507,8 @@
     <cellStyle name="Hyperlink for amounts" xfId="25"/>
     <cellStyle name="Hyperlnk row header underlined bold" xfId="26"/>
     <cellStyle name="Middle Headers Centered" xfId="27"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Norm." xfId="0" builtinId="0"/>
+    <cellStyle name="Otsikko" xfId="3" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Placeholder" xfId="28"/>
     <cellStyle name="Placeholder Header Underlined bold" xfId="29"/>
     <cellStyle name="Placeholder_column_blank" xfId="30"/>
@@ -510,7 +521,8 @@
     <cellStyle name="Subtotal head row fill" xfId="37"/>
     <cellStyle name="Subtotal_amounts" xfId="38"/>
     <cellStyle name="TGK_TOC_PAGE_COLUMN" xfId="39"/>
-    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Valuutta" xfId="1" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Valuutta [0]" xfId="2" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Visual Check" xfId="40"/>
     <cellStyle name="Webdings" xfId="41"/>
     <cellStyle name="Webdings1" xfId="42"/>
@@ -518,7 +530,251 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="35">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top style="thin">
+          <color auto="1"/>
+        </top>
+        <bottom style="thin">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -856,12 +1112,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1"/>
+  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -869,27 +1125,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:E23"/>
+  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="64.5703125" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="46.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="64.5" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="46.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -898,99 +1154,107 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
       <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
         <v>3</v>
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" t="s">
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" t="s">
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
@@ -1018,13 +1282,11 @@
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15 D14">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="C14:E16">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"borderless"</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>"border"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Error message more talkative #39
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
+++ b/vaadin-spreadsheet/src/test/resources/test_sheets/conditional_formatting_with_formula_on_second_sheet.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mtzukanov/IdeaProjects/tagetik-2017-spreadsheet/vaadin-spreadsheet/src/test/resources/test_sheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\svn\GIT\tagetik-2017-spreadsheet\vaadin-spreadsheet\src\test\resources\test_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="660" windowWidth="26400" windowHeight="15740" activeTab="1"/>
+    <workbookView xWindow="12660" yWindow="660" windowWidth="26400" windowHeight="15735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -21,11 +21,11 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -500,6 +500,8 @@
     <cellStyle name="Bold+Italic" xfId="18"/>
     <cellStyle name="C_Amount_ACT" xfId="19"/>
     <cellStyle name="C_Head" xfId="20"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4" customBuiltin="1"/>
+    <cellStyle name="Currency [0]" xfId="2" builtinId="7" customBuiltin="1"/>
     <cellStyle name="Date" xfId="21"/>
     <cellStyle name="Fill light blue" xfId="22"/>
     <cellStyle name="Formula" xfId="23"/>
@@ -507,8 +509,7 @@
     <cellStyle name="Hyperlink for amounts" xfId="25"/>
     <cellStyle name="Hyperlnk row header underlined bold" xfId="26"/>
     <cellStyle name="Middle Headers Centered" xfId="27"/>
-    <cellStyle name="Norm." xfId="0" builtinId="0"/>
-    <cellStyle name="Otsikko" xfId="3" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Placeholder" xfId="28"/>
     <cellStyle name="Placeholder Header Underlined bold" xfId="29"/>
     <cellStyle name="Placeholder_column_blank" xfId="30"/>
@@ -521,8 +522,7 @@
     <cellStyle name="Subtotal head row fill" xfId="37"/>
     <cellStyle name="Subtotal_amounts" xfId="38"/>
     <cellStyle name="TGK_TOC_PAGE_COLUMN" xfId="39"/>
-    <cellStyle name="Valuutta" xfId="1" builtinId="4" customBuiltin="1"/>
-    <cellStyle name="Valuutta [0]" xfId="2" builtinId="7" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="3" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Visual Check" xfId="40"/>
     <cellStyle name="Webdings" xfId="41"/>
     <cellStyle name="Webdings1" xfId="42"/>
@@ -530,190 +530,7 @@
     <cellStyle name="Work new book placeholder header underlined" xfId="44"/>
     <cellStyle name="WrappedText" xfId="45"/>
   </cellStyles>
-  <dxfs count="35">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="14">
     <dxf>
       <border>
         <left style="thin">
@@ -1112,12 +929,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1125,27 +942,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Sheet2" enableFormatConditionsCalculation="0"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="64.5" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="46.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="64.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="7" max="7" width="46.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -1154,46 +971,46 @@
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="C14" s="4"/>
       <c r="D14" s="3"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="C15" s="3"/>
       <c r="D15" s="4" t="s">
@@ -1201,7 +1018,7 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
@@ -1209,84 +1026,84 @@
       </c>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" s="7"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="13" priority="7">
       <formula>($A$1=A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="9" priority="3">
       <formula>-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14:E16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
       <formula>"borderless"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>"border"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20494,7 +20311,7 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
@@ -20506,7 +20323,7 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B0EC025-287A-42C9-90F3-9FD04AC8F706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4B01778-499A-4DF4-B495-12FA425BE2FF}">
   <ds:schemaRefs/>
 </ds:datastoreItem>
 </file>
</xml_diff>